<commit_message>
Auswertung zum Befüllungsgrad relevanter Attribute
</commit_message>
<xml_diff>
--- a/survey-results-schema.xlsx
+++ b/survey-results-schema.xlsx
@@ -8,14 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://porsche-my.sharepoint.com/personal/oliver_balb_porsche_de/Documents/Documents/_Orga/96 - Training/DataScience/04 Data Scientist/3C2S/DS3BP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="8_{5A9206A6-C9EF-478F-B2F2-18FA90736B62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10FB9A62-D07E-4B22-87E9-E0CE15AA1B98}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="8_{5A9206A6-C9EF-478F-B2F2-18FA90736B62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B23F7257-46B3-48EC-8A9B-85A56EDB59EF}"/>
   <bookViews>
-    <workbookView xWindow="-27990" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey-results-schema (2)" sheetId="2" r:id="rId1"/>
     <sheet name="survey-results-schema" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'survey-results-schema (2)'!$A$1:$D$157</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -34,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="492">
   <si>
     <t>Column,Question</t>
   </si>
@@ -1438,13 +1442,85 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>Relevance</t>
+  </si>
+  <si>
+    <t>'YearsProgram',</t>
+  </si>
+  <si>
+    <t>'YearsCodedJob',</t>
+  </si>
+  <si>
+    <t>'DeveloperType',</t>
+  </si>
+  <si>
+    <t>'WebDeveloperType',</t>
+  </si>
+  <si>
+    <t>'MobileDeveloperType',</t>
+  </si>
+  <si>
+    <t>'NonDeveloperType',</t>
+  </si>
+  <si>
+    <t>'ProblemSolving',</t>
+  </si>
+  <si>
+    <t>'BuildingThings',</t>
+  </si>
+  <si>
+    <t>'LearningNewTech',</t>
+  </si>
+  <si>
+    <t>'BoringDetails',</t>
+  </si>
+  <si>
+    <t>'FriendsDevelopers',</t>
+  </si>
+  <si>
+    <t>'RightWrongWay',</t>
+  </si>
+  <si>
+    <t>'UnderstandComputers',</t>
+  </si>
+  <si>
+    <t>'SeriousWork',</t>
+  </si>
+  <si>
+    <t>'InvestTimeTools',</t>
+  </si>
+  <si>
+    <t>'ChallengeMyself',</t>
+  </si>
+  <si>
+    <t>'CompetePeers',</t>
+  </si>
+  <si>
+    <t>'ChangeWorld',</t>
+  </si>
+  <si>
+    <t>'HaveWorkedLanguage',</t>
+  </si>
+  <si>
+    <t>'WantWorkLanguage',</t>
+  </si>
+  <si>
+    <t>'HaveWorkedFramework',</t>
+  </si>
+  <si>
+    <t>'WantWorkFramework',</t>
+  </si>
+  <si>
+    <t>'HighestEducationParents',</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1559,6 +1635,12 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Porsche Next TT"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
       <name val="Porsche Next TT"/>
       <family val="2"/>
     </font>
@@ -1904,8 +1986,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2261,26 +2349,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:D157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B94" sqref="B94"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13:D150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="51.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="51.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="91" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
         <v>159</v>
       </c>
@@ -2288,7 +2383,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B3" t="s">
         <v>161</v>
       </c>
@@ -2296,7 +2391,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
         <v>163</v>
       </c>
@@ -2304,7 +2399,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
         <v>165</v>
       </c>
@@ -2312,7 +2407,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
         <v>167</v>
       </c>
@@ -2320,7 +2415,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:4" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B7" t="s">
         <v>169</v>
       </c>
@@ -2328,7 +2423,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:4" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
         <v>171</v>
       </c>
@@ -2336,7 +2431,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:4" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B9" t="s">
         <v>173</v>
       </c>
@@ -2344,7 +2439,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:4" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B10" t="s">
         <v>175</v>
       </c>
@@ -2352,7 +2447,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:4" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B11" t="s">
         <v>177</v>
       </c>
@@ -2360,7 +2455,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:4" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B12" t="s">
         <v>179</v>
       </c>
@@ -2368,29 +2463,37 @@
         <v>180</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A13" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A13" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="2" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A14" t="s">
+      <c r="D13" s="1" t="str">
+        <f>"'" &amp; B13 &amp; "',"</f>
+        <v>'YearsProgram',</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A14" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="2" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D14" s="1" t="str">
+        <f>"'" &amp; B14 &amp; "',"</f>
+        <v>'YearsCodedJob',</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B15" t="s">
         <v>185</v>
       </c>
@@ -2398,51 +2501,67 @@
         <v>186</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A16" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A16" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="2" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A17" t="s">
+      <c r="D16" s="1" t="str">
+        <f t="shared" ref="D16:D19" si="0">"'" &amp; B16 &amp; "',"</f>
+        <v>'DeveloperType',</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A17" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="2" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A18" t="s">
+      <c r="D17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>'WebDeveloperType',</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A18" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A19" t="s">
+      <c r="D18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>'MobileDeveloperType',</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A19" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="2" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>'NonDeveloperType',</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B20" t="s">
         <v>195</v>
       </c>
@@ -2450,7 +2569,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B21" t="s">
         <v>197</v>
       </c>
@@ -2458,7 +2577,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B22" t="s">
         <v>199</v>
       </c>
@@ -2466,7 +2585,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:4" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B23" t="s">
         <v>201</v>
       </c>
@@ -2474,7 +2593,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:4" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B24" t="s">
         <v>203</v>
       </c>
@@ -2482,7 +2601,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:4" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B25" t="s">
         <v>205</v>
       </c>
@@ -2490,7 +2609,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:4" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B26" t="s">
         <v>207</v>
       </c>
@@ -2498,7 +2617,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:4" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B27" t="s">
         <v>209</v>
       </c>
@@ -2506,7 +2625,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:4" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B28" t="s">
         <v>211</v>
       </c>
@@ -2514,7 +2633,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:4" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B29" t="s">
         <v>213</v>
       </c>
@@ -2522,7 +2641,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:4" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B30" t="s">
         <v>215</v>
       </c>
@@ -2530,48 +2649,67 @@
         <v>216</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A31" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A31" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="2" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A32" t="s">
+      <c r="D31" s="1" t="str">
+        <f t="shared" ref="D31:D34" si="1">"'" &amp; B31 &amp; "',"</f>
+        <v>'ProblemSolving',</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A32" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="2" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A33" t="s">
+      <c r="D32" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>'BuildingThings',</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A33" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="2" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B34" t="s">
+      <c r="D33" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>'LearningNewTech',</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A34" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="2" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D34" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>'BoringDetails',</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B35" t="s">
         <v>225</v>
       </c>
@@ -2579,7 +2717,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:4" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B36" t="s">
         <v>227</v>
       </c>
@@ -2587,7 +2725,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:4" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B37" t="s">
         <v>229</v>
       </c>
@@ -2595,56 +2733,82 @@
         <v>230</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B38" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A38" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="2" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B39" t="s">
+      <c r="D38" s="1" t="str">
+        <f t="shared" ref="D38:D42" si="2">"'" &amp; B38 &amp; "',"</f>
+        <v>'FriendsDevelopers',</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A39" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="2" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A40" t="s">
+      <c r="D39" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>'RightWrongWay',</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A40" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="2" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A41" t="s">
+      <c r="D40" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>'UnderstandComputers',</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A41" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="2" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A42" t="s">
+      <c r="D41" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>'SeriousWork',</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A42" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="2" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D42" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>'InvestTimeTools',</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B43" t="s">
         <v>241</v>
       </c>
@@ -2652,7 +2816,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:4" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B44" t="s">
         <v>243</v>
       </c>
@@ -2660,37 +2824,52 @@
         <v>244</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A45" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A45" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="2" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A46" t="s">
+      <c r="D45" s="1" t="str">
+        <f t="shared" ref="D45:D47" si="3">"'" &amp; B45 &amp; "',"</f>
+        <v>'ChallengeMyself',</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A46" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="2" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B47" t="s">
+      <c r="D46" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>'CompetePeers',</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A47" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="2" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D47" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>'ChangeWorld',</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B48" t="s">
         <v>251</v>
       </c>
@@ -2698,7 +2877,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="49" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B49" t="s">
         <v>253</v>
       </c>
@@ -2706,7 +2885,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="50" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B50" t="s">
         <v>255</v>
       </c>
@@ -2714,7 +2893,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="51" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B51" t="s">
         <v>257</v>
       </c>
@@ -2722,7 +2901,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="52" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B52" t="s">
         <v>259</v>
       </c>
@@ -2730,7 +2909,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="53" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B53" t="s">
         <v>261</v>
       </c>
@@ -2738,7 +2917,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="54" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B54" t="s">
         <v>263</v>
       </c>
@@ -2746,7 +2925,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="55" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B55" t="s">
         <v>265</v>
       </c>
@@ -2754,7 +2933,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="56" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B56" t="s">
         <v>267</v>
       </c>
@@ -2762,7 +2941,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="57" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B57" t="s">
         <v>269</v>
       </c>
@@ -2770,7 +2949,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="58" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B58" t="s">
         <v>271</v>
       </c>
@@ -2778,7 +2957,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="59" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B59" t="s">
         <v>273</v>
       </c>
@@ -2786,7 +2965,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="60" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B60" t="s">
         <v>275</v>
       </c>
@@ -2794,7 +2973,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="61" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B61" t="s">
         <v>277</v>
       </c>
@@ -2802,7 +2981,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="62" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B62" t="s">
         <v>279</v>
       </c>
@@ -2810,7 +2989,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="63" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B63" t="s">
         <v>281</v>
       </c>
@@ -2818,7 +2997,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="64" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B64" t="s">
         <v>283</v>
       </c>
@@ -2826,7 +3005,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="65" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B65" t="s">
         <v>285</v>
       </c>
@@ -2834,7 +3013,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="66" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B66" t="s">
         <v>287</v>
       </c>
@@ -2842,7 +3021,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="67" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B67" t="s">
         <v>289</v>
       </c>
@@ -2850,7 +3029,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="68" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B68" t="s">
         <v>291</v>
       </c>
@@ -2858,7 +3037,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="69" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B69" t="s">
         <v>293</v>
       </c>
@@ -2866,7 +3045,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="70" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B70" t="s">
         <v>295</v>
       </c>
@@ -2874,7 +3053,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="71" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B71" t="s">
         <v>297</v>
       </c>
@@ -2882,7 +3061,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="72" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B72" t="s">
         <v>299</v>
       </c>
@@ -2890,7 +3069,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="73" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B73" t="s">
         <v>301</v>
       </c>
@@ -2898,7 +3077,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="74" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B74" t="s">
         <v>303</v>
       </c>
@@ -2906,7 +3085,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="75" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B75" t="s">
         <v>305</v>
       </c>
@@ -2914,7 +3093,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="76" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B76" t="s">
         <v>307</v>
       </c>
@@ -2922,7 +3101,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="77" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B77" t="s">
         <v>309</v>
       </c>
@@ -2930,7 +3109,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="78" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B78" t="s">
         <v>311</v>
       </c>
@@ -2938,7 +3117,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="79" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="79" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B79" t="s">
         <v>313</v>
       </c>
@@ -2946,7 +3125,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="80" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B80" t="s">
         <v>315</v>
       </c>
@@ -2954,7 +3133,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:4" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B81" t="s">
         <v>317</v>
       </c>
@@ -2962,7 +3141,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:4" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B82" t="s">
         <v>319</v>
       </c>
@@ -2970,7 +3149,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:4" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B83" t="s">
         <v>321</v>
       </c>
@@ -2978,7 +3157,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:4" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B84" t="s">
         <v>323</v>
       </c>
@@ -2986,7 +3165,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:4" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B85" t="s">
         <v>325</v>
       </c>
@@ -2994,7 +3173,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:4" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B86" t="s">
         <v>327</v>
       </c>
@@ -3002,7 +3181,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:4" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B87" t="s">
         <v>329</v>
       </c>
@@ -3010,7 +3189,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:4" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B88" t="s">
         <v>331</v>
       </c>
@@ -3018,7 +3197,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:4" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B89" t="s">
         <v>333</v>
       </c>
@@ -3029,7 +3208,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:4" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B90" t="s">
         <v>336</v>
       </c>
@@ -3040,7 +3219,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:4" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B91" t="s">
         <v>338</v>
       </c>
@@ -3049,50 +3228,66 @@
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A92" t="s">
+      <c r="A92" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B92" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C92" s="2" t="s">
         <v>341</v>
       </c>
+      <c r="D92" s="1" t="str">
+        <f t="shared" ref="D92:D95" si="4">"'" &amp; B92 &amp; "',"</f>
+        <v>'HaveWorkedLanguage',</v>
+      </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A93" t="s">
+      <c r="A93" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B93" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C93" s="2" t="s">
         <v>341</v>
       </c>
+      <c r="D93" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>'WantWorkLanguage',</v>
+      </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A94" t="s">
+      <c r="A94" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B94" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C94" s="2" t="s">
         <v>344</v>
       </c>
+      <c r="D94" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>'HaveWorkedFramework',</v>
+      </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A95" t="s">
+      <c r="A95" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B95" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C95" s="2" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="D95" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>'WantWorkFramework',</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B96" t="s">
         <v>346</v>
       </c>
@@ -3100,7 +3295,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="97" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B97" t="s">
         <v>348</v>
       </c>
@@ -3108,7 +3303,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="98" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B98" t="s">
         <v>349</v>
       </c>
@@ -3116,7 +3311,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="99" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B99" t="s">
         <v>351</v>
       </c>
@@ -3124,7 +3319,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="100" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B100" t="s">
         <v>352</v>
       </c>
@@ -3132,7 +3327,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="101" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="101" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B101" t="s">
         <v>354</v>
       </c>
@@ -3140,7 +3335,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="102" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="102" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B102" t="s">
         <v>356</v>
       </c>
@@ -3148,7 +3343,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="103" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="103" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B103" t="s">
         <v>358</v>
       </c>
@@ -3156,7 +3351,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="104" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="104" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B104" t="s">
         <v>360</v>
       </c>
@@ -3164,7 +3359,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="105" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="105" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B105" t="s">
         <v>362</v>
       </c>
@@ -3172,7 +3367,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="106" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="106" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B106" t="s">
         <v>364</v>
       </c>
@@ -3180,7 +3375,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="107" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="107" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B107" t="s">
         <v>366</v>
       </c>
@@ -3188,7 +3383,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="108" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="108" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B108" t="s">
         <v>368</v>
       </c>
@@ -3196,7 +3391,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="109" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="109" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B109" t="s">
         <v>370</v>
       </c>
@@ -3204,7 +3399,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="110" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="110" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B110" t="s">
         <v>372</v>
       </c>
@@ -3212,7 +3407,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="111" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="111" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B111" t="s">
         <v>374</v>
       </c>
@@ -3220,7 +3415,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="112" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="112" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B112" t="s">
         <v>376</v>
       </c>
@@ -3228,7 +3423,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="113" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="113" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B113" t="s">
         <v>378</v>
       </c>
@@ -3236,7 +3431,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="114" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="114" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B114" t="s">
         <v>380</v>
       </c>
@@ -3244,7 +3439,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="115" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="115" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B115" t="s">
         <v>382</v>
       </c>
@@ -3252,7 +3447,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="116" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="116" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B116" t="s">
         <v>384</v>
       </c>
@@ -3260,7 +3455,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="117" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="117" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B117" t="s">
         <v>386</v>
       </c>
@@ -3268,7 +3463,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="118" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="118" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B118" t="s">
         <v>388</v>
       </c>
@@ -3276,7 +3471,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="119" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="119" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B119" t="s">
         <v>390</v>
       </c>
@@ -3284,7 +3479,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="120" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="120" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B120" t="s">
         <v>392</v>
       </c>
@@ -3292,7 +3487,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="121" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="121" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B121" t="s">
         <v>394</v>
       </c>
@@ -3300,7 +3495,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="122" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="122" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B122" t="s">
         <v>396</v>
       </c>
@@ -3308,7 +3503,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="123" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="123" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B123" t="s">
         <v>398</v>
       </c>
@@ -3316,7 +3511,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="124" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="124" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B124" t="s">
         <v>400</v>
       </c>
@@ -3324,7 +3519,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="125" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="125" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B125" t="s">
         <v>402</v>
       </c>
@@ -3332,7 +3527,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="126" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="126" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B126" t="s">
         <v>404</v>
       </c>
@@ -3340,7 +3535,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="127" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="127" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B127" t="s">
         <v>406</v>
       </c>
@@ -3348,7 +3543,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="128" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="128" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B128" t="s">
         <v>408</v>
       </c>
@@ -3356,7 +3551,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="129" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="129" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B129" t="s">
         <v>410</v>
       </c>
@@ -3364,7 +3559,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="130" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="130" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B130" t="s">
         <v>412</v>
       </c>
@@ -3372,7 +3567,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="131" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="131" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B131" t="s">
         <v>413</v>
       </c>
@@ -3380,7 +3575,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="132" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="132" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B132" t="s">
         <v>415</v>
       </c>
@@ -3388,7 +3583,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="133" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="133" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B133" t="s">
         <v>417</v>
       </c>
@@ -3396,7 +3591,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="134" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="134" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B134" t="s">
         <v>419</v>
       </c>
@@ -3404,7 +3599,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="135" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="135" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B135" t="s">
         <v>421</v>
       </c>
@@ -3412,7 +3607,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="136" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="136" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B136" t="s">
         <v>423</v>
       </c>
@@ -3420,7 +3615,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="137" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="137" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B137" t="s">
         <v>425</v>
       </c>
@@ -3428,7 +3623,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="138" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="138" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B138" t="s">
         <v>427</v>
       </c>
@@ -3436,7 +3631,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="139" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="139" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B139" t="s">
         <v>429</v>
       </c>
@@ -3444,7 +3639,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="140" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="140" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B140" t="s">
         <v>431</v>
       </c>
@@ -3452,7 +3647,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="141" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="141" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B141" t="s">
         <v>433</v>
       </c>
@@ -3460,7 +3655,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="142" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="142" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B142" t="s">
         <v>435</v>
       </c>
@@ -3468,7 +3663,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="143" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="143" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B143" t="s">
         <v>437</v>
       </c>
@@ -3476,7 +3671,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="144" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="144" spans="2:3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B144" t="s">
         <v>439</v>
       </c>
@@ -3484,7 +3679,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="145" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="145" spans="1:4" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B145" t="s">
         <v>441</v>
       </c>
@@ -3492,7 +3687,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="146" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="146" spans="1:4" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B146" t="s">
         <v>443</v>
       </c>
@@ -3500,7 +3695,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="147" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="147" spans="1:4" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B147" t="s">
         <v>445</v>
       </c>
@@ -3508,7 +3703,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="148" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="148" spans="1:4" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B148" t="s">
         <v>447</v>
       </c>
@@ -3516,7 +3711,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="149" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="149" spans="1:4" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B149" t="s">
         <v>449</v>
       </c>
@@ -3524,15 +3719,22 @@
         <v>450</v>
       </c>
     </row>
-    <row r="150" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B150" t="s">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A150" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="B150" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="C150" t="s">
+      <c r="C150" s="2" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="151" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="D150" s="1" t="str">
+        <f t="shared" ref="D150" si="5">"'" &amp; B150 &amp; "',"</f>
+        <v>'HighestEducationParents',</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B151" t="s">
         <v>453</v>
       </c>
@@ -3540,7 +3742,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="152" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="152" spans="1:4" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B152" t="s">
         <v>455</v>
       </c>
@@ -3548,7 +3750,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="153" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="153" spans="1:4" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B153" t="s">
         <v>457</v>
       </c>
@@ -3556,7 +3758,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="154" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="154" spans="1:4" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B154" t="s">
         <v>459</v>
       </c>
@@ -3564,7 +3766,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="155" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="155" spans="1:4" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B155" t="s">
         <v>461</v>
       </c>
@@ -3572,7 +3774,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="156" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="156" spans="1:4" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B156" t="s">
         <v>463</v>
       </c>
@@ -3580,7 +3782,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="157" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="157" spans="1:4" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="B157" t="s">
         <v>465</v>
       </c>
@@ -3589,6 +3791,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D157" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4391,4 +4600,90 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{990AAE54-9A3F-44DA-AFDB-AF3796E83DDE}">
+  <dimension ref="A1:W1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:W1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>469</v>
+      </c>
+      <c r="B1" t="s">
+        <v>470</v>
+      </c>
+      <c r="C1" t="s">
+        <v>471</v>
+      </c>
+      <c r="D1" t="s">
+        <v>472</v>
+      </c>
+      <c r="E1" t="s">
+        <v>473</v>
+      </c>
+      <c r="F1" t="s">
+        <v>474</v>
+      </c>
+      <c r="G1" t="s">
+        <v>475</v>
+      </c>
+      <c r="H1" t="s">
+        <v>476</v>
+      </c>
+      <c r="I1" t="s">
+        <v>477</v>
+      </c>
+      <c r="J1" t="s">
+        <v>478</v>
+      </c>
+      <c r="K1" t="s">
+        <v>479</v>
+      </c>
+      <c r="L1" t="s">
+        <v>480</v>
+      </c>
+      <c r="M1" t="s">
+        <v>481</v>
+      </c>
+      <c r="N1" t="s">
+        <v>482</v>
+      </c>
+      <c r="O1" t="s">
+        <v>483</v>
+      </c>
+      <c r="P1" t="s">
+        <v>484</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>485</v>
+      </c>
+      <c r="R1" t="s">
+        <v>486</v>
+      </c>
+      <c r="S1" t="s">
+        <v>487</v>
+      </c>
+      <c r="T1" t="s">
+        <v>488</v>
+      </c>
+      <c r="U1" t="s">
+        <v>489</v>
+      </c>
+      <c r="V1" t="s">
+        <v>490</v>
+      </c>
+      <c r="W1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>